<commit_message>
CP04OSPM Caland ingest sheets dep 3
Reviewed ingest and cal sheets

changed reference designator for MOPAK in Cal sheet for dep 3 and
created ingest sheet for deployment 3
</commit_message>
<xml_diff>
--- a/CP04OSPM/Omaha_Cal_Info_CP04OSPM_00003.xlsx
+++ b/CP04OSPM/Omaha_Cal_Info_CP04OSPM_00003.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="10700" windowWidth="24820" windowHeight="11280" tabRatio="377"/>
+    <workbookView xWindow="10860" yWindow="10695" windowWidth="24825" windowHeight="11280" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$83</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$398</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -230,9 +230,6 @@
     <t>CP04OSPM-WFP01-00-WFPENG000</t>
   </si>
   <si>
-    <t>CP04OSPM-SBS01-01-MOPAK0000</t>
-  </si>
-  <si>
     <t>CC_angular_resolution</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>OSPM-00003-MOPAK</t>
+  </si>
+  <si>
+    <t>CP04OSPM-SBS11-02-MOPAK0000</t>
   </si>
 </sst>
 </file>
@@ -279,7 +279,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -385,26 +385,36 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -427,7 +437,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -489,6 +499,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -518,7 +541,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -601,6 +624,9 @@
     </xf>
     <xf numFmtId="11" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="26">
@@ -1002,22 +1028,22 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="10" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="10" width="16.85546875" customWidth="1"/>
     <col min="11" max="11" width="44" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:13" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,12 +1078,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15">
+    <row r="2" spans="1:13">
       <c r="A2" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="23">
         <v>3</v>
@@ -1072,16 +1098,16 @@
         <v>42289</v>
       </c>
       <c r="G2" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>61</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>62</v>
       </c>
       <c r="I2" s="23">
         <v>436</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="11"/>
@@ -1108,24 +1134,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="41.6640625" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="14" max="14" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:14" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1145,18 +1172,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:14" ht="15" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="13">
         <v>3</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>16</v>
@@ -1169,18 +1196,18 @@
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:14" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="13">
         <v>3</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>14</v>
@@ -1191,18 +1218,18 @@
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:14" ht="15" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="13">
         <v>3</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>15</v>
@@ -1213,18 +1240,18 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:14" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="13">
         <v>3</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>17</v>
@@ -1237,18 +1264,18 @@
       </c>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:14" ht="15" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="13">
         <v>3</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>18</v>
@@ -1261,18 +1288,18 @@
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:14" ht="15" customHeight="1">
       <c r="A7" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="13">
         <v>3</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>19</v>
@@ -1285,18 +1312,18 @@
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="13">
         <v>3</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>20</v>
@@ -1309,18 +1336,18 @@
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:14" ht="15" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="13">
         <v>3</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>21</v>
@@ -1333,7 +1360,7 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:14" ht="15" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1342,13 +1369,14 @@
       <c r="F10" s="14"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="N10" s="33"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1">
       <c r="A11" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="13">
         <v>3</v>
@@ -1364,13 +1392,14 @@
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="N11" s="33"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="13">
         <v>3</v>
@@ -1386,8 +1415,9 @@
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="N12" s="33"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1396,13 +1426,14 @@
       <c r="F13" s="15"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="N13" s="33"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" customHeight="1">
       <c r="A14" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="13">
         <v>3</v>
@@ -1418,13 +1449,14 @@
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="N14" s="33"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" customHeight="1">
       <c r="A15" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="13">
         <v>3</v>
@@ -1440,8 +1472,9 @@
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="N15" s="33"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" customHeight="1">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -1451,12 +1484,12 @@
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="15" customHeight="1">
       <c r="A17" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="13">
         <v>3</v>
@@ -1465,7 +1498,7 @@
         <v>1118</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" s="18">
         <v>1.0760000000000001</v>
@@ -1475,12 +1508,12 @@
       </c>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="15" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="13">
         <v>3</v>
@@ -1499,12 +1532,12 @@
       </c>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="15" customHeight="1">
       <c r="A19" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="13">
         <v>3</v>
@@ -1523,12 +1556,12 @@
       </c>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="15" customHeight="1">
       <c r="A20" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="13">
         <v>3</v>
@@ -1547,12 +1580,12 @@
       </c>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="15" customHeight="1">
       <c r="A21" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="13">
         <v>3</v>
@@ -1561,7 +1594,7 @@
         <v>1118</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="19">
         <v>3.9E-2</v>
@@ -1571,12 +1604,12 @@
       </c>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="15" customHeight="1">
       <c r="A22" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="13">
         <v>3</v>
@@ -1585,7 +1618,7 @@
         <v>1118</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" s="19">
         <v>700</v>
@@ -1595,12 +1628,12 @@
       </c>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="15" customHeight="1">
       <c r="A23" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="13">
         <v>3</v>
@@ -1619,12 +1652,12 @@
       </c>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="15" customHeight="1">
       <c r="A24" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="13">
         <v>3</v>
@@ -1643,12 +1676,12 @@
       </c>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="15" customHeight="1">
       <c r="A25" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="13">
         <v>3</v>
@@ -1667,12 +1700,12 @@
       </c>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="15" customHeight="1">
       <c r="A26" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="13">
         <v>3</v>
@@ -1681,7 +1714,7 @@
         <v>1118</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26" s="18">
         <v>124</v>
@@ -1691,7 +1724,7 @@
       </c>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="15" customHeight="1">
       <c r="A27" s="12"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1701,12 +1734,12 @@
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="15" customHeight="1">
       <c r="A28" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="13">
         <v>3</v>
@@ -1725,12 +1758,12 @@
       </c>
       <c r="H28" s="12"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="15" customHeight="1">
       <c r="A29" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="13">
         <v>3</v>
@@ -1749,7 +1782,7 @@
       </c>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="15" customHeight="1">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -1759,25 +1792,25 @@
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" ht="15" customHeight="1">
       <c r="A31" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="13">
         <v>3</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="17"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" ht="15" customHeight="1">
       <c r="A32" s="12"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -1787,18 +1820,18 @@
       <c r="G32" s="17"/>
       <c r="H32" s="12"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="15" customHeight="1">
       <c r="A33" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="13">
         <v>3</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="16"/>
@@ -1807,7 +1840,7 @@
       </c>
       <c r="H33" s="12"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="15" customHeight="1">
       <c r="A34" s="12"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -1817,18 +1850,18 @@
       <c r="G34" s="17"/>
       <c r="H34" s="12"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="15" customHeight="1">
       <c r="A35" s="12" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" s="13">
         <v>3</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
@@ -1837,11 +1870,11 @@
       </c>
       <c r="H35" s="12"/>
     </row>
-    <row r="36" spans="1:8" ht="15">
+    <row r="36" spans="1:8" ht="15" customHeight="1">
       <c r="A36" s="6"/>
       <c r="D36" s="22"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="15" customHeight="1">
       <c r="D37" s="22"/>
     </row>
   </sheetData>

</xml_diff>